<commit_message>
datos pacientes lista de espera a archivo .dat
</commit_message>
<xml_diff>
--- a/Libro2.xlsx
+++ b/Libro2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RESPALDO\Desktop\Grafos\Waiting-list-optimization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -13,7 +18,7 @@
     <sheet name="jueves" sheetId="4" r:id="rId4"/>
     <sheet name="viernes" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1628,8 +1633,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1692,11 +1697,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1738,7 +1751,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1770,9 +1783,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1804,6 +1818,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1979,14 +1994,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2021,7 +2038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2056,7 +2073,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -2091,7 +2108,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11</v>
       </c>
@@ -2126,7 +2143,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -2161,7 +2178,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2196,7 +2213,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13</v>
       </c>
@@ -2231,7 +2248,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2266,7 +2283,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -2301,7 +2318,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -2336,7 +2353,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -2371,7 +2388,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -2406,7 +2423,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2441,7 +2458,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2476,7 +2493,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -2511,7 +2528,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -2546,7 +2563,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2581,7 +2598,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -2616,7 +2633,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -2651,7 +2668,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2686,7 +2703,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -2721,7 +2738,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
@@ -2756,7 +2773,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2791,7 +2808,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
@@ -2826,7 +2843,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
@@ -2861,7 +2878,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14</v>
       </c>
@@ -2896,7 +2913,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>14</v>
       </c>
@@ -2931,7 +2948,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2966,7 +2983,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3001,7 +3018,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3036,7 +3053,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>14</v>
       </c>
@@ -3071,7 +3088,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3106,7 +3123,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -3141,7 +3158,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3176,7 +3193,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -3211,7 +3228,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -3246,7 +3263,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
@@ -3281,7 +3298,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>13</v>
       </c>
@@ -3316,7 +3333,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>12</v>
       </c>
@@ -3351,7 +3368,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -3386,7 +3403,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3421,7 +3438,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
@@ -3456,7 +3473,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>10</v>
       </c>
@@ -3491,7 +3508,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3526,7 +3543,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>8</v>
       </c>
@@ -3561,7 +3578,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>8</v>
       </c>
@@ -3602,14 +3619,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3644,7 +3661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>13</v>
       </c>
@@ -3679,7 +3696,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -3714,7 +3731,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -3749,7 +3766,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -3784,7 +3801,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -3819,7 +3836,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3854,7 +3871,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -3889,7 +3906,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -3924,7 +3941,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
@@ -3959,7 +3976,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3994,7 +4011,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -4029,7 +4046,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -4064,7 +4081,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -4099,7 +4116,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -4134,7 +4151,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -4169,7 +4186,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -4204,7 +4221,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -4239,7 +4256,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -4274,7 +4291,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
@@ -4309,7 +4326,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -4344,7 +4361,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -4379,7 +4396,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -4414,7 +4431,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -4449,7 +4466,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -4484,7 +4501,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -4519,7 +4536,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -4554,7 +4571,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -4589,7 +4606,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -4624,7 +4641,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -4659,7 +4676,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -4694,7 +4711,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -4729,7 +4746,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10</v>
       </c>
@@ -4764,7 +4781,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -4799,7 +4816,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>13</v>
       </c>
@@ -4834,7 +4851,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -4869,7 +4886,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>14</v>
       </c>
@@ -4910,14 +4927,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4952,7 +4969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -4987,7 +5004,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5022,7 +5039,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -5057,7 +5074,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -5092,7 +5109,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -5127,7 +5144,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -5162,7 +5179,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5197,7 +5214,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5232,7 +5249,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5267,7 +5284,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -5302,7 +5319,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -5337,7 +5354,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -5372,7 +5389,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -5407,7 +5424,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -5442,7 +5459,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -5477,7 +5494,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -5512,7 +5529,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5547,7 +5564,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
@@ -5582,7 +5599,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -5617,7 +5634,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -5652,7 +5669,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -5687,7 +5704,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -5722,7 +5739,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -5757,7 +5774,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -5792,7 +5809,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11</v>
       </c>
@@ -5827,7 +5844,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -5862,7 +5879,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -5897,7 +5914,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
@@ -5932,7 +5949,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -5967,7 +5984,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>11</v>
       </c>
@@ -6002,7 +6019,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
@@ -6037,7 +6054,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -6072,7 +6089,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -6107,7 +6124,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10</v>
       </c>
@@ -6142,7 +6159,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8</v>
       </c>
@@ -6177,7 +6194,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -6212,7 +6229,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -6253,14 +6270,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6295,7 +6312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -6330,7 +6347,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -6365,7 +6382,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6400,7 +6417,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -6435,7 +6452,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>12</v>
       </c>
@@ -6470,7 +6487,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -6505,7 +6522,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -6540,7 +6557,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6575,7 +6592,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -6610,7 +6627,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -6645,7 +6662,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -6680,7 +6697,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -6715,7 +6732,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -6750,7 +6767,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -6785,7 +6802,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -6820,7 +6837,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -6855,7 +6872,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -6890,7 +6907,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -6925,7 +6942,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -6960,7 +6977,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -6995,7 +7012,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
@@ -7030,7 +7047,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -7065,7 +7082,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -7100,7 +7117,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>9</v>
       </c>
@@ -7135,7 +7152,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -7170,7 +7187,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -7205,7 +7222,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14</v>
       </c>
@@ -7240,7 +7257,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -7275,7 +7292,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -7310,7 +7327,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -7345,7 +7362,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12</v>
       </c>
@@ -7380,7 +7397,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -7415,7 +7432,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -7450,7 +7467,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -7485,7 +7502,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10</v>
       </c>
@@ -7520,7 +7537,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -7555,7 +7572,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -7590,7 +7607,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -7631,14 +7648,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7673,7 +7690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -7708,7 +7725,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14</v>
       </c>
@@ -7743,7 +7760,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -7778,7 +7795,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -7813,7 +7830,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -7848,7 +7865,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13</v>
       </c>
@@ -7883,7 +7900,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -7918,7 +7935,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -7953,7 +7970,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -7988,7 +8005,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -8023,7 +8040,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8058,7 +8075,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -8093,7 +8110,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -8128,7 +8145,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -8163,7 +8180,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -8198,7 +8215,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -8233,7 +8250,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -8268,7 +8285,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -8303,7 +8320,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -8338,7 +8355,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -8373,7 +8390,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -8408,7 +8425,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12</v>
       </c>
@@ -8443,7 +8460,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -8478,7 +8495,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
@@ -8513,7 +8530,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>13</v>
       </c>
@@ -8548,7 +8565,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>
@@ -8583,7 +8600,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>13</v>
       </c>
@@ -8618,7 +8635,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -8653,7 +8670,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8</v>
       </c>
@@ -8688,7 +8705,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8</v>
       </c>
@@ -8723,7 +8740,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>14</v>
       </c>
@@ -8758,7 +8775,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -8793,7 +8810,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>12</v>
       </c>
@@ -8828,7 +8845,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -8863,7 +8880,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -8898,7 +8915,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>11</v>
       </c>
@@ -8933,7 +8950,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>13</v>
       </c>

</xml_diff>